<commit_message>
Implemented ChangePassword and Manage Lisitings feature
</commit_message>
<xml_diff>
--- a/AdvancedTaskPart2_UserStory1.xlsx
+++ b/AdvancedTaskPart2_UserStory1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\post2\Desktop\MVP_Studio\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01E12E7-24B3-48DD-990F-B2124AF2E643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841A7B0F-7852-4D1A-BD4F-FA62B2D67CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{368EC0D6-A85F-4759-84BB-F1E98E940A91}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="191">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -158,17 +158,10 @@
     <t>AdvancedTask Part 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user can able to change password </t>
-  </si>
-  <si>
     <t>"Password changed successfully" should be displayed</t>
   </si>
   <si>
     <t>"Password changed successfully" is displayed</t>
-  </si>
-  <si>
-    <t>1.Click Change Password under Hi Username tab
-2.Enter current password, new password and confirm password and click save button.</t>
   </si>
   <si>
     <t>Current password - Selenium@2
@@ -660,6 +653,52 @@
   <si>
     <t>Request button is disabled.
 Not able to send requests</t>
+  </si>
+  <si>
+    <t>"Password Verification Failed" should be displayed</t>
+  </si>
+  <si>
+    <t>"Password Verification Failed" is displayed</t>
+  </si>
+  <si>
+    <t>Current password - qwert
+New password - Selenium
+Confirm password - Selenium</t>
+  </si>
+  <si>
+    <t>Verify that user can enter invalid current password while attempting to change the password</t>
+  </si>
+  <si>
+    <t>Verify that user can enter valid details while attempting to change the password</t>
+  </si>
+  <si>
+    <t>1.Click Change Password under Hi Username tab
+2.Enter valid current password, new password and confirm password and click save button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify  change password </t>
+  </si>
+  <si>
+    <t>Verify that the new password and Confirm password does not match</t>
+  </si>
+  <si>
+    <t>1.Click Change Password under Hi Username tab
+2.Enter invalid current password 3.Enter valid new password and confirm password and click save button.</t>
+  </si>
+  <si>
+    <t>1.Click Change Password under Hi Username tab
+2.Enter valid current password 3.Enter new password and different confirm password and click save button.</t>
+  </si>
+  <si>
+    <t>Current password - Selenium@2
+New password - qwerty
+Confirm password - Specflow</t>
+  </si>
+  <si>
+    <t>"Password does not match" should be displayed</t>
+  </si>
+  <si>
+    <t>"Password does not match" is displayed</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC586CD-4AE2-4478-A6E4-1FBB36125457}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,7 +1121,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1146,18 +1185,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>43</v>
+        <v>182</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
@@ -1166,33 +1205,29 @@
         <v>12</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>46</v>
+        <v>183</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>57</v>
-      </c>
+    </row>
+    <row r="11" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>48</v>
+        <v>181</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
@@ -1201,250 +1236,250 @@
         <v>12</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
+        <v>186</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>50</v>
+        <v>178</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>52</v>
+        <v>185</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="244.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>79</v>
-      </c>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="244.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>11</v>
@@ -1453,223 +1488,289 @@
         <v>12</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="C20" s="2" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="196.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="H23" s="3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>115</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="196.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="2" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="3"/>
+      <c r="C26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1739,13 +1840,13 @@
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -1754,19 +1855,19 @@
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1776,7 +1877,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
@@ -1785,19 +1886,19 @@
         <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1807,7 +1908,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
@@ -1816,19 +1917,19 @@
         <v>12</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1836,13 +1937,13 @@
         <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -1851,19 +1952,19 @@
         <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1873,7 +1974,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -1882,19 +1983,19 @@
         <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1902,34 +2003,34 @@
         <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2013,13 +2114,13 @@
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -2028,19 +2129,19 @@
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2050,7 +2151,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
@@ -2059,19 +2160,19 @@
         <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
@@ -2081,7 +2182,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
@@ -2090,19 +2191,19 @@
         <v>12</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2112,7 +2213,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -2121,19 +2222,19 @@
         <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2141,13 +2242,13 @@
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -2156,19 +2257,19 @@
         <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2178,7 +2279,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
@@ -2187,19 +2288,19 @@
         <v>12</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>